<commit_message>
store changes for osprey eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeachefr.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeachefr.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62390458-DDC6-4E9F-A4F1-20647A8A352E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB899727-6B78-492A-9911-959D4CAD0B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="900" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="304">
   <si>
     <t>UserName</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t>skasarla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>One Size</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDE721-2994-4A91-8C89-FADAE76105D8}">
   <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,7 +1878,7 @@
         <v>280</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>206</v>
+        <v>303</v>
       </c>
       <c r="V3" t="s">
         <v>100</v>
@@ -4912,8 +4915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B006AB-898C-4D28-9BA9-3207EC054E17}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5052,7 +5055,7 @@
         <v>297</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>206</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>